<commit_message>
Computed results for world 3
</commit_message>
<xml_diff>
--- a/results/WorldUnknown/MeansAndSTDCont.xlsx
+++ b/results/WorldUnknown/MeansAndSTDCont.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M151"/>
+  <dimension ref="A1:M232"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
@@ -9330,6 +9330,4785 @@
         </is>
       </c>
     </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B152" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C152" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D152" t="n">
+        <v>100</v>
+      </c>
+      <c r="E152" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>-0.075</t>
+        </is>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>0.044</t>
+        </is>
+      </c>
+      <c r="H152" t="inlineStr">
+        <is>
+          <t>-0.054</t>
+        </is>
+      </c>
+      <c r="I152" t="inlineStr">
+        <is>
+          <t>0.075</t>
+        </is>
+      </c>
+      <c r="J152" t="inlineStr">
+        <is>
+          <t>-0.048</t>
+        </is>
+      </c>
+      <c r="K152" t="inlineStr">
+        <is>
+          <t>0.082</t>
+        </is>
+      </c>
+      <c r="L152" t="inlineStr">
+        <is>
+          <t>-0.060</t>
+        </is>
+      </c>
+      <c r="M152" t="inlineStr">
+        <is>
+          <t>0.067</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B153" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C153" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D153" t="n">
+        <v>50</v>
+      </c>
+      <c r="E153" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>-0.083</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>0.043</t>
+        </is>
+      </c>
+      <c r="H153" t="inlineStr">
+        <is>
+          <t>-0.089</t>
+        </is>
+      </c>
+      <c r="I153" t="inlineStr">
+        <is>
+          <t>0.031</t>
+        </is>
+      </c>
+      <c r="J153" t="inlineStr">
+        <is>
+          <t>-0.041</t>
+        </is>
+      </c>
+      <c r="K153" t="inlineStr">
+        <is>
+          <t>0.092</t>
+        </is>
+      </c>
+      <c r="L153" t="inlineStr">
+        <is>
+          <t>-0.078</t>
+        </is>
+      </c>
+      <c r="M153" t="inlineStr">
+        <is>
+          <t>0.060</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B154" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C154" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D154" t="n">
+        <v>100</v>
+      </c>
+      <c r="E154" t="n">
+        <v>1</v>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>-0.056</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>0.052</t>
+        </is>
+      </c>
+      <c r="H154" t="inlineStr">
+        <is>
+          <t>-0.059</t>
+        </is>
+      </c>
+      <c r="I154" t="inlineStr">
+        <is>
+          <t>0.051</t>
+        </is>
+      </c>
+      <c r="J154" t="inlineStr">
+        <is>
+          <t>-0.058</t>
+        </is>
+      </c>
+      <c r="K154" t="inlineStr">
+        <is>
+          <t>0.055</t>
+        </is>
+      </c>
+      <c r="L154" t="inlineStr">
+        <is>
+          <t>-0.063</t>
+        </is>
+      </c>
+      <c r="M154" t="inlineStr">
+        <is>
+          <t>0.042</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B155" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C155" t="n">
+        <v>1</v>
+      </c>
+      <c r="D155" t="n">
+        <v>100</v>
+      </c>
+      <c r="E155" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>-0.079</t>
+        </is>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>0.041</t>
+        </is>
+      </c>
+      <c r="H155" t="inlineStr">
+        <is>
+          <t>-0.057</t>
+        </is>
+      </c>
+      <c r="I155" t="inlineStr">
+        <is>
+          <t>0.066</t>
+        </is>
+      </c>
+      <c r="J155" t="inlineStr">
+        <is>
+          <t>-0.070</t>
+        </is>
+      </c>
+      <c r="K155" t="inlineStr">
+        <is>
+          <t>0.053</t>
+        </is>
+      </c>
+      <c r="L155" t="inlineStr">
+        <is>
+          <t>-0.051</t>
+        </is>
+      </c>
+      <c r="M155" t="inlineStr">
+        <is>
+          <t>0.069</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B156" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C156" t="n">
+        <v>1</v>
+      </c>
+      <c r="D156" t="n">
+        <v>100</v>
+      </c>
+      <c r="E156" t="n">
+        <v>1</v>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>-0.048</t>
+        </is>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>0.070</t>
+        </is>
+      </c>
+      <c r="H156" t="inlineStr">
+        <is>
+          <t>-0.051</t>
+        </is>
+      </c>
+      <c r="I156" t="inlineStr">
+        <is>
+          <t>0.060</t>
+        </is>
+      </c>
+      <c r="J156" t="inlineStr">
+        <is>
+          <t>-0.052</t>
+        </is>
+      </c>
+      <c r="K156" t="inlineStr">
+        <is>
+          <t>0.062</t>
+        </is>
+      </c>
+      <c r="L156" t="inlineStr">
+        <is>
+          <t>-0.051</t>
+        </is>
+      </c>
+      <c r="M156" t="inlineStr">
+        <is>
+          <t>0.062</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B157" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C157" t="n">
+        <v>1</v>
+      </c>
+      <c r="D157" t="n">
+        <v>50</v>
+      </c>
+      <c r="E157" t="n">
+        <v>1</v>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>-0.062</t>
+        </is>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>0.060</t>
+        </is>
+      </c>
+      <c r="H157" t="inlineStr">
+        <is>
+          <t>-0.067</t>
+        </is>
+      </c>
+      <c r="I157" t="inlineStr">
+        <is>
+          <t>0.061</t>
+        </is>
+      </c>
+      <c r="J157" t="inlineStr">
+        <is>
+          <t>-0.073</t>
+        </is>
+      </c>
+      <c r="K157" t="inlineStr">
+        <is>
+          <t>0.042</t>
+        </is>
+      </c>
+      <c r="L157" t="inlineStr">
+        <is>
+          <t>-0.077</t>
+        </is>
+      </c>
+      <c r="M157" t="inlineStr">
+        <is>
+          <t>0.042</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B158" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C158" t="n">
+        <v>1</v>
+      </c>
+      <c r="D158" t="n">
+        <v>100</v>
+      </c>
+      <c r="E158" t="n">
+        <v>5</v>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>-0.046</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>0.077</t>
+        </is>
+      </c>
+      <c r="H158" t="inlineStr">
+        <is>
+          <t>-0.037</t>
+        </is>
+      </c>
+      <c r="I158" t="inlineStr">
+        <is>
+          <t>0.092</t>
+        </is>
+      </c>
+      <c r="J158" t="inlineStr">
+        <is>
+          <t>-0.085</t>
+        </is>
+      </c>
+      <c r="K158" t="inlineStr">
+        <is>
+          <t>0.026</t>
+        </is>
+      </c>
+      <c r="L158" t="inlineStr">
+        <is>
+          <t>-0.091</t>
+        </is>
+      </c>
+      <c r="M158" t="inlineStr">
+        <is>
+          <t>0.033</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B159" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C159" t="n">
+        <v>1</v>
+      </c>
+      <c r="D159" t="n">
+        <v>50</v>
+      </c>
+      <c r="E159" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>-0.049</t>
+        </is>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>0.084</t>
+        </is>
+      </c>
+      <c r="H159" t="inlineStr">
+        <is>
+          <t>-0.069</t>
+        </is>
+      </c>
+      <c r="I159" t="inlineStr">
+        <is>
+          <t>0.068</t>
+        </is>
+      </c>
+      <c r="J159" t="inlineStr">
+        <is>
+          <t>-0.086</t>
+        </is>
+      </c>
+      <c r="K159" t="inlineStr">
+        <is>
+          <t>0.037</t>
+        </is>
+      </c>
+      <c r="L159" t="inlineStr">
+        <is>
+          <t>-0.086</t>
+        </is>
+      </c>
+      <c r="M159" t="inlineStr">
+        <is>
+          <t>0.045</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B160" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C160" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D160" t="n">
+        <v>50</v>
+      </c>
+      <c r="E160" t="n">
+        <v>5</v>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>-0.096</t>
+        </is>
+      </c>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>0.018</t>
+        </is>
+      </c>
+      <c r="H160" t="inlineStr">
+        <is>
+          <t>-0.033</t>
+        </is>
+      </c>
+      <c r="I160" t="inlineStr">
+        <is>
+          <t>0.102</t>
+        </is>
+      </c>
+      <c r="J160" t="inlineStr">
+        <is>
+          <t>-0.068</t>
+        </is>
+      </c>
+      <c r="K160" t="inlineStr">
+        <is>
+          <t>0.077</t>
+        </is>
+      </c>
+      <c r="L160" t="inlineStr">
+        <is>
+          <t>-0.080</t>
+        </is>
+      </c>
+      <c r="M160" t="inlineStr">
+        <is>
+          <t>0.059</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B161" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C161" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D161" t="n">
+        <v>100</v>
+      </c>
+      <c r="E161" t="n">
+        <v>5</v>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>-0.061</t>
+        </is>
+      </c>
+      <c r="G161" t="inlineStr">
+        <is>
+          <t>0.073</t>
+        </is>
+      </c>
+      <c r="H161" t="inlineStr">
+        <is>
+          <t>-0.088</t>
+        </is>
+      </c>
+      <c r="I161" t="inlineStr">
+        <is>
+          <t>0.038</t>
+        </is>
+      </c>
+      <c r="J161" t="inlineStr">
+        <is>
+          <t>-0.083</t>
+        </is>
+      </c>
+      <c r="K161" t="inlineStr">
+        <is>
+          <t>0.060</t>
+        </is>
+      </c>
+      <c r="L161" t="inlineStr">
+        <is>
+          <t>-0.046</t>
+        </is>
+      </c>
+      <c r="M161" t="inlineStr">
+        <is>
+          <t>0.086</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B162" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C162" t="n">
+        <v>1</v>
+      </c>
+      <c r="D162" t="n">
+        <v>50</v>
+      </c>
+      <c r="E162" t="n">
+        <v>5</v>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>-0.049</t>
+        </is>
+      </c>
+      <c r="G162" t="inlineStr">
+        <is>
+          <t>0.093</t>
+        </is>
+      </c>
+      <c r="H162" t="inlineStr">
+        <is>
+          <t>-0.089</t>
+        </is>
+      </c>
+      <c r="I162" t="inlineStr">
+        <is>
+          <t>0.039</t>
+        </is>
+      </c>
+      <c r="J162" t="inlineStr">
+        <is>
+          <t>-0.092</t>
+        </is>
+      </c>
+      <c r="K162" t="inlineStr">
+        <is>
+          <t>0.025</t>
+        </is>
+      </c>
+      <c r="L162" t="inlineStr">
+        <is>
+          <t>-0.084</t>
+        </is>
+      </c>
+      <c r="M162" t="inlineStr">
+        <is>
+          <t>0.058</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B163" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C163" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D163" t="n">
+        <v>50</v>
+      </c>
+      <c r="E163" t="n">
+        <v>1</v>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>-0.081</t>
+        </is>
+      </c>
+      <c r="G163" t="inlineStr">
+        <is>
+          <t>0.041</t>
+        </is>
+      </c>
+      <c r="H163" t="inlineStr">
+        <is>
+          <t>-0.071</t>
+        </is>
+      </c>
+      <c r="I163" t="inlineStr">
+        <is>
+          <t>0.056</t>
+        </is>
+      </c>
+      <c r="J163" t="inlineStr">
+        <is>
+          <t>-0.069</t>
+        </is>
+      </c>
+      <c r="K163" t="inlineStr">
+        <is>
+          <t>0.053</t>
+        </is>
+      </c>
+      <c r="L163" t="inlineStr">
+        <is>
+          <t>-0.061</t>
+        </is>
+      </c>
+      <c r="M163" t="inlineStr">
+        <is>
+          <t>0.063</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B164" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C164" t="n">
+        <v>1</v>
+      </c>
+      <c r="D164" t="n">
+        <v>10</v>
+      </c>
+      <c r="E164" t="n">
+        <v>5</v>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>-0.094</t>
+        </is>
+      </c>
+      <c r="G164" t="inlineStr">
+        <is>
+          <t>0.033</t>
+        </is>
+      </c>
+      <c r="H164" t="inlineStr">
+        <is>
+          <t>-0.096</t>
+        </is>
+      </c>
+      <c r="I164" t="inlineStr">
+        <is>
+          <t>0.017</t>
+        </is>
+      </c>
+      <c r="J164" t="inlineStr">
+        <is>
+          <t>-0.092</t>
+        </is>
+      </c>
+      <c r="K164" t="inlineStr">
+        <is>
+          <t>0.039</t>
+        </is>
+      </c>
+      <c r="L164" t="inlineStr">
+        <is>
+          <t>-0.098</t>
+        </is>
+      </c>
+      <c r="M164" t="inlineStr">
+        <is>
+          <t>0.014</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B165" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C165" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D165" t="n">
+        <v>10</v>
+      </c>
+      <c r="E165" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>-0.093</t>
+        </is>
+      </c>
+      <c r="G165" t="inlineStr">
+        <is>
+          <t>0.037</t>
+        </is>
+      </c>
+      <c r="H165" t="inlineStr">
+        <is>
+          <t>-0.086</t>
+        </is>
+      </c>
+      <c r="I165" t="inlineStr">
+        <is>
+          <t>0.050</t>
+        </is>
+      </c>
+      <c r="J165" t="inlineStr">
+        <is>
+          <t>-0.095</t>
+        </is>
+      </c>
+      <c r="K165" t="inlineStr">
+        <is>
+          <t>0.029</t>
+        </is>
+      </c>
+      <c r="L165" t="inlineStr">
+        <is>
+          <t>-0.096</t>
+        </is>
+      </c>
+      <c r="M165" t="inlineStr">
+        <is>
+          <t>0.032</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B166" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C166" t="n">
+        <v>1</v>
+      </c>
+      <c r="D166" t="n">
+        <v>10</v>
+      </c>
+      <c r="E166" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>-0.095</t>
+        </is>
+      </c>
+      <c r="G166" t="inlineStr">
+        <is>
+          <t>0.026</t>
+        </is>
+      </c>
+      <c r="H166" t="inlineStr">
+        <is>
+          <t>-0.097</t>
+        </is>
+      </c>
+      <c r="I166" t="inlineStr">
+        <is>
+          <t>0.020</t>
+        </is>
+      </c>
+      <c r="J166" t="inlineStr">
+        <is>
+          <t>-0.096</t>
+        </is>
+      </c>
+      <c r="K166" t="inlineStr">
+        <is>
+          <t>0.019</t>
+        </is>
+      </c>
+      <c r="L166" t="inlineStr">
+        <is>
+          <t>-0.095</t>
+        </is>
+      </c>
+      <c r="M166" t="inlineStr">
+        <is>
+          <t>0.029</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B167" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C167" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D167" t="n">
+        <v>10</v>
+      </c>
+      <c r="E167" t="n">
+        <v>5</v>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>-0.096</t>
+        </is>
+      </c>
+      <c r="G167" t="inlineStr">
+        <is>
+          <t>0.019</t>
+        </is>
+      </c>
+      <c r="H167" t="inlineStr">
+        <is>
+          <t>-0.097</t>
+        </is>
+      </c>
+      <c r="I167" t="inlineStr">
+        <is>
+          <t>0.022</t>
+        </is>
+      </c>
+      <c r="J167" t="inlineStr">
+        <is>
+          <t>-0.057</t>
+        </is>
+      </c>
+      <c r="K167" t="inlineStr">
+        <is>
+          <t>0.089</t>
+        </is>
+      </c>
+      <c r="L167" t="inlineStr">
+        <is>
+          <t>-0.097</t>
+        </is>
+      </c>
+      <c r="M167" t="inlineStr">
+        <is>
+          <t>0.012</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B168" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C168" t="n">
+        <v>1</v>
+      </c>
+      <c r="D168" t="n">
+        <v>10</v>
+      </c>
+      <c r="E168" t="n">
+        <v>1</v>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>-0.093</t>
+        </is>
+      </c>
+      <c r="G168" t="inlineStr">
+        <is>
+          <t>0.024</t>
+        </is>
+      </c>
+      <c r="H168" t="inlineStr">
+        <is>
+          <t>-0.085</t>
+        </is>
+      </c>
+      <c r="I168" t="inlineStr">
+        <is>
+          <t>0.054</t>
+        </is>
+      </c>
+      <c r="J168" t="inlineStr">
+        <is>
+          <t>-0.080</t>
+        </is>
+      </c>
+      <c r="K168" t="inlineStr">
+        <is>
+          <t>0.058</t>
+        </is>
+      </c>
+      <c r="L168" t="inlineStr">
+        <is>
+          <t>-0.082</t>
+        </is>
+      </c>
+      <c r="M168" t="inlineStr">
+        <is>
+          <t>0.049</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B169" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C169" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D169" t="n">
+        <v>10</v>
+      </c>
+      <c r="E169" t="n">
+        <v>1</v>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>-0.094</t>
+        </is>
+      </c>
+      <c r="G169" t="inlineStr">
+        <is>
+          <t>0.026</t>
+        </is>
+      </c>
+      <c r="H169" t="inlineStr">
+        <is>
+          <t>-0.080</t>
+        </is>
+      </c>
+      <c r="I169" t="inlineStr">
+        <is>
+          <t>0.056</t>
+        </is>
+      </c>
+      <c r="J169" t="inlineStr">
+        <is>
+          <t>-0.085</t>
+        </is>
+      </c>
+      <c r="K169" t="inlineStr">
+        <is>
+          <t>0.050</t>
+        </is>
+      </c>
+      <c r="L169" t="inlineStr">
+        <is>
+          <t>-0.090</t>
+        </is>
+      </c>
+      <c r="M169" t="inlineStr">
+        <is>
+          <t>0.049</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B170" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C170" t="n">
+        <v>5</v>
+      </c>
+      <c r="D170" t="n">
+        <v>100</v>
+      </c>
+      <c r="E170" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>-0.054</t>
+        </is>
+      </c>
+      <c r="G170" t="inlineStr">
+        <is>
+          <t>0.072</t>
+        </is>
+      </c>
+      <c r="H170" t="inlineStr">
+        <is>
+          <t>-0.046</t>
+        </is>
+      </c>
+      <c r="I170" t="inlineStr">
+        <is>
+          <t>0.076</t>
+        </is>
+      </c>
+      <c r="J170" t="inlineStr">
+        <is>
+          <t>-0.061</t>
+        </is>
+      </c>
+      <c r="K170" t="inlineStr">
+        <is>
+          <t>0.064</t>
+        </is>
+      </c>
+      <c r="L170" t="inlineStr">
+        <is>
+          <t>-0.046</t>
+        </is>
+      </c>
+      <c r="M170" t="inlineStr">
+        <is>
+          <t>0.076</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B171" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C171" t="n">
+        <v>5</v>
+      </c>
+      <c r="D171" t="n">
+        <v>100</v>
+      </c>
+      <c r="E171" t="n">
+        <v>5</v>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>-0.086</t>
+        </is>
+      </c>
+      <c r="G171" t="inlineStr">
+        <is>
+          <t>0.042</t>
+        </is>
+      </c>
+      <c r="H171" t="inlineStr">
+        <is>
+          <t>-0.054</t>
+        </is>
+      </c>
+      <c r="I171" t="inlineStr">
+        <is>
+          <t>0.078</t>
+        </is>
+      </c>
+      <c r="J171" t="inlineStr">
+        <is>
+          <t>-0.057</t>
+        </is>
+      </c>
+      <c r="K171" t="inlineStr">
+        <is>
+          <t>0.074</t>
+        </is>
+      </c>
+      <c r="L171" t="inlineStr">
+        <is>
+          <t>-0.050</t>
+        </is>
+      </c>
+      <c r="M171" t="inlineStr">
+        <is>
+          <t>0.084</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B172" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C172" t="n">
+        <v>5</v>
+      </c>
+      <c r="D172" t="n">
+        <v>100</v>
+      </c>
+      <c r="E172" t="n">
+        <v>1</v>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>-0.052</t>
+        </is>
+      </c>
+      <c r="G172" t="inlineStr">
+        <is>
+          <t>0.053</t>
+        </is>
+      </c>
+      <c r="H172" t="inlineStr">
+        <is>
+          <t>-0.055</t>
+        </is>
+      </c>
+      <c r="I172" t="inlineStr">
+        <is>
+          <t>0.059</t>
+        </is>
+      </c>
+      <c r="J172" t="inlineStr">
+        <is>
+          <t>-0.048</t>
+        </is>
+      </c>
+      <c r="K172" t="inlineStr">
+        <is>
+          <t>0.071</t>
+        </is>
+      </c>
+      <c r="L172" t="inlineStr">
+        <is>
+          <t>-0.052</t>
+        </is>
+      </c>
+      <c r="M172" t="inlineStr">
+        <is>
+          <t>0.063</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B173" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C173" t="n">
+        <v>1</v>
+      </c>
+      <c r="D173" t="n">
+        <v>100</v>
+      </c>
+      <c r="E173" t="n">
+        <v>5</v>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>-0.087</t>
+        </is>
+      </c>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>0.047</t>
+        </is>
+      </c>
+      <c r="H173" t="inlineStr">
+        <is>
+          <t>-0.080</t>
+        </is>
+      </c>
+      <c r="I173" t="inlineStr">
+        <is>
+          <t>0.054</t>
+        </is>
+      </c>
+      <c r="J173" t="inlineStr">
+        <is>
+          <t>-0.077</t>
+        </is>
+      </c>
+      <c r="K173" t="inlineStr">
+        <is>
+          <t>0.050</t>
+        </is>
+      </c>
+      <c r="L173" t="inlineStr">
+        <is>
+          <t>-0.086</t>
+        </is>
+      </c>
+      <c r="M173" t="inlineStr">
+        <is>
+          <t>0.036</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B174" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C174" t="n">
+        <v>1</v>
+      </c>
+      <c r="D174" t="n">
+        <v>100</v>
+      </c>
+      <c r="E174" t="n">
+        <v>1</v>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>-0.052</t>
+        </is>
+      </c>
+      <c r="G174" t="inlineStr">
+        <is>
+          <t>0.073</t>
+        </is>
+      </c>
+      <c r="H174" t="inlineStr">
+        <is>
+          <t>-0.048</t>
+        </is>
+      </c>
+      <c r="I174" t="inlineStr">
+        <is>
+          <t>0.075</t>
+        </is>
+      </c>
+      <c r="J174" t="inlineStr">
+        <is>
+          <t>-0.054</t>
+        </is>
+      </c>
+      <c r="K174" t="inlineStr">
+        <is>
+          <t>0.071</t>
+        </is>
+      </c>
+      <c r="L174" t="inlineStr">
+        <is>
+          <t>-0.066</t>
+        </is>
+      </c>
+      <c r="M174" t="inlineStr">
+        <is>
+          <t>0.043</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B175" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C175" t="n">
+        <v>5</v>
+      </c>
+      <c r="D175" t="n">
+        <v>50</v>
+      </c>
+      <c r="E175" t="n">
+        <v>5</v>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>-0.087</t>
+        </is>
+      </c>
+      <c r="G175" t="inlineStr">
+        <is>
+          <t>0.051</t>
+        </is>
+      </c>
+      <c r="H175" t="inlineStr">
+        <is>
+          <t>-0.078</t>
+        </is>
+      </c>
+      <c r="I175" t="inlineStr">
+        <is>
+          <t>0.062</t>
+        </is>
+      </c>
+      <c r="J175" t="inlineStr">
+        <is>
+          <t>-0.093</t>
+        </is>
+      </c>
+      <c r="K175" t="inlineStr">
+        <is>
+          <t>0.033</t>
+        </is>
+      </c>
+      <c r="L175" t="inlineStr">
+        <is>
+          <t>-0.091</t>
+        </is>
+      </c>
+      <c r="M175" t="inlineStr">
+        <is>
+          <t>0.033</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B176" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C176" t="n">
+        <v>1</v>
+      </c>
+      <c r="D176" t="n">
+        <v>100</v>
+      </c>
+      <c r="E176" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>-0.059</t>
+        </is>
+      </c>
+      <c r="G176" t="inlineStr">
+        <is>
+          <t>0.058</t>
+        </is>
+      </c>
+      <c r="H176" t="inlineStr">
+        <is>
+          <t>-0.082</t>
+        </is>
+      </c>
+      <c r="I176" t="inlineStr">
+        <is>
+          <t>0.043</t>
+        </is>
+      </c>
+      <c r="J176" t="inlineStr">
+        <is>
+          <t>-0.080</t>
+        </is>
+      </c>
+      <c r="K176" t="inlineStr">
+        <is>
+          <t>0.052</t>
+        </is>
+      </c>
+      <c r="L176" t="inlineStr">
+        <is>
+          <t>-0.086</t>
+        </is>
+      </c>
+      <c r="M176" t="inlineStr">
+        <is>
+          <t>0.036</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B177" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C177" t="n">
+        <v>5</v>
+      </c>
+      <c r="D177" t="n">
+        <v>50</v>
+      </c>
+      <c r="E177" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>-0.049</t>
+        </is>
+      </c>
+      <c r="G177" t="inlineStr">
+        <is>
+          <t>0.086</t>
+        </is>
+      </c>
+      <c r="H177" t="inlineStr">
+        <is>
+          <t>-0.074</t>
+        </is>
+      </c>
+      <c r="I177" t="inlineStr">
+        <is>
+          <t>0.054</t>
+        </is>
+      </c>
+      <c r="J177" t="inlineStr">
+        <is>
+          <t>-0.049</t>
+        </is>
+      </c>
+      <c r="K177" t="inlineStr">
+        <is>
+          <t>0.086</t>
+        </is>
+      </c>
+      <c r="L177" t="inlineStr">
+        <is>
+          <t>-0.082</t>
+        </is>
+      </c>
+      <c r="M177" t="inlineStr">
+        <is>
+          <t>0.043</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B178" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C178" t="n">
+        <v>1</v>
+      </c>
+      <c r="D178" t="n">
+        <v>50</v>
+      </c>
+      <c r="E178" t="n">
+        <v>1</v>
+      </c>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>-0.076</t>
+        </is>
+      </c>
+      <c r="G178" t="inlineStr">
+        <is>
+          <t>0.049</t>
+        </is>
+      </c>
+      <c r="H178" t="inlineStr">
+        <is>
+          <t>-0.069</t>
+        </is>
+      </c>
+      <c r="I178" t="inlineStr">
+        <is>
+          <t>0.062</t>
+        </is>
+      </c>
+      <c r="J178" t="inlineStr">
+        <is>
+          <t>-0.075</t>
+        </is>
+      </c>
+      <c r="K178" t="inlineStr">
+        <is>
+          <t>0.060</t>
+        </is>
+      </c>
+      <c r="L178" t="inlineStr">
+        <is>
+          <t>-0.069</t>
+        </is>
+      </c>
+      <c r="M178" t="inlineStr">
+        <is>
+          <t>0.062</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B179" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C179" t="n">
+        <v>1</v>
+      </c>
+      <c r="D179" t="n">
+        <v>10</v>
+      </c>
+      <c r="E179" t="n">
+        <v>5</v>
+      </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>-0.093</t>
+        </is>
+      </c>
+      <c r="G179" t="inlineStr">
+        <is>
+          <t>0.032</t>
+        </is>
+      </c>
+      <c r="H179" t="inlineStr">
+        <is>
+          <t>-0.096</t>
+        </is>
+      </c>
+      <c r="I179" t="inlineStr">
+        <is>
+          <t>0.036</t>
+        </is>
+      </c>
+      <c r="J179" t="inlineStr">
+        <is>
+          <t>-0.094</t>
+        </is>
+      </c>
+      <c r="K179" t="inlineStr">
+        <is>
+          <t>0.031</t>
+        </is>
+      </c>
+      <c r="L179" t="inlineStr">
+        <is>
+          <t>-0.092</t>
+        </is>
+      </c>
+      <c r="M179" t="inlineStr">
+        <is>
+          <t>0.039</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B180" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C180" t="n">
+        <v>1</v>
+      </c>
+      <c r="D180" t="n">
+        <v>50</v>
+      </c>
+      <c r="E180" t="n">
+        <v>5</v>
+      </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>-0.094</t>
+        </is>
+      </c>
+      <c r="G180" t="inlineStr">
+        <is>
+          <t>0.028</t>
+        </is>
+      </c>
+      <c r="H180" t="inlineStr">
+        <is>
+          <t>-0.087</t>
+        </is>
+      </c>
+      <c r="I180" t="inlineStr">
+        <is>
+          <t>0.048</t>
+        </is>
+      </c>
+      <c r="J180" t="inlineStr">
+        <is>
+          <t>-0.095</t>
+        </is>
+      </c>
+      <c r="K180" t="inlineStr">
+        <is>
+          <t>0.023</t>
+        </is>
+      </c>
+      <c r="L180" t="inlineStr">
+        <is>
+          <t>-0.095</t>
+        </is>
+      </c>
+      <c r="M180" t="inlineStr">
+        <is>
+          <t>0.017</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B181" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C181" t="n">
+        <v>1</v>
+      </c>
+      <c r="D181" t="n">
+        <v>50</v>
+      </c>
+      <c r="E181" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F181" t="inlineStr">
+        <is>
+          <t>-0.061</t>
+        </is>
+      </c>
+      <c r="G181" t="inlineStr">
+        <is>
+          <t>0.071</t>
+        </is>
+      </c>
+      <c r="H181" t="inlineStr">
+        <is>
+          <t>-0.079</t>
+        </is>
+      </c>
+      <c r="I181" t="inlineStr">
+        <is>
+          <t>0.058</t>
+        </is>
+      </c>
+      <c r="J181" t="inlineStr">
+        <is>
+          <t>-0.093</t>
+        </is>
+      </c>
+      <c r="K181" t="inlineStr">
+        <is>
+          <t>0.024</t>
+        </is>
+      </c>
+      <c r="L181" t="inlineStr">
+        <is>
+          <t>-0.086</t>
+        </is>
+      </c>
+      <c r="M181" t="inlineStr">
+        <is>
+          <t>0.039</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B182" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C182" t="n">
+        <v>1</v>
+      </c>
+      <c r="D182" t="n">
+        <v>10</v>
+      </c>
+      <c r="E182" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>-0.094</t>
+        </is>
+      </c>
+      <c r="G182" t="inlineStr">
+        <is>
+          <t>0.022</t>
+        </is>
+      </c>
+      <c r="H182" t="inlineStr">
+        <is>
+          <t>-0.078</t>
+        </is>
+      </c>
+      <c r="I182" t="inlineStr">
+        <is>
+          <t>0.068</t>
+        </is>
+      </c>
+      <c r="J182" t="inlineStr">
+        <is>
+          <t>-0.095</t>
+        </is>
+      </c>
+      <c r="K182" t="inlineStr">
+        <is>
+          <t>0.025</t>
+        </is>
+      </c>
+      <c r="L182" t="inlineStr">
+        <is>
+          <t>-0.090</t>
+        </is>
+      </c>
+      <c r="M182" t="inlineStr">
+        <is>
+          <t>0.051</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B183" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C183" t="n">
+        <v>5</v>
+      </c>
+      <c r="D183" t="n">
+        <v>10</v>
+      </c>
+      <c r="E183" t="n">
+        <v>5</v>
+      </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>-0.096</t>
+        </is>
+      </c>
+      <c r="G183" t="inlineStr">
+        <is>
+          <t>0.029</t>
+        </is>
+      </c>
+      <c r="H183" t="inlineStr">
+        <is>
+          <t>-0.095</t>
+        </is>
+      </c>
+      <c r="I183" t="inlineStr">
+        <is>
+          <t>0.025</t>
+        </is>
+      </c>
+      <c r="J183" t="inlineStr">
+        <is>
+          <t>-0.098</t>
+        </is>
+      </c>
+      <c r="K183" t="inlineStr">
+        <is>
+          <t>0.010</t>
+        </is>
+      </c>
+      <c r="L183" t="inlineStr">
+        <is>
+          <t>-0.096</t>
+        </is>
+      </c>
+      <c r="M183" t="inlineStr">
+        <is>
+          <t>0.024</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B184" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C184" t="n">
+        <v>5</v>
+      </c>
+      <c r="D184" t="n">
+        <v>10</v>
+      </c>
+      <c r="E184" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>-0.092</t>
+        </is>
+      </c>
+      <c r="G184" t="inlineStr">
+        <is>
+          <t>0.028</t>
+        </is>
+      </c>
+      <c r="H184" t="inlineStr">
+        <is>
+          <t>-0.092</t>
+        </is>
+      </c>
+      <c r="I184" t="inlineStr">
+        <is>
+          <t>0.035</t>
+        </is>
+      </c>
+      <c r="J184" t="inlineStr">
+        <is>
+          <t>-0.096</t>
+        </is>
+      </c>
+      <c r="K184" t="inlineStr">
+        <is>
+          <t>0.027</t>
+        </is>
+      </c>
+      <c r="L184" t="inlineStr">
+        <is>
+          <t>-0.068</t>
+        </is>
+      </c>
+      <c r="M184" t="inlineStr">
+        <is>
+          <t>0.081</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B185" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C185" t="n">
+        <v>5</v>
+      </c>
+      <c r="D185" t="n">
+        <v>50</v>
+      </c>
+      <c r="E185" t="n">
+        <v>1</v>
+      </c>
+      <c r="F185" t="inlineStr">
+        <is>
+          <t>-0.066</t>
+        </is>
+      </c>
+      <c r="G185" t="inlineStr">
+        <is>
+          <t>0.058</t>
+        </is>
+      </c>
+      <c r="H185" t="inlineStr">
+        <is>
+          <t>-0.074</t>
+        </is>
+      </c>
+      <c r="I185" t="inlineStr">
+        <is>
+          <t>0.061</t>
+        </is>
+      </c>
+      <c r="J185" t="inlineStr">
+        <is>
+          <t>-0.052</t>
+        </is>
+      </c>
+      <c r="K185" t="inlineStr">
+        <is>
+          <t>0.078</t>
+        </is>
+      </c>
+      <c r="L185" t="inlineStr">
+        <is>
+          <t>-0.061</t>
+        </is>
+      </c>
+      <c r="M185" t="inlineStr">
+        <is>
+          <t>0.062</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B186" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C186" t="n">
+        <v>1</v>
+      </c>
+      <c r="D186" t="n">
+        <v>10</v>
+      </c>
+      <c r="E186" t="n">
+        <v>1</v>
+      </c>
+      <c r="F186" t="inlineStr">
+        <is>
+          <t>-0.078</t>
+        </is>
+      </c>
+      <c r="G186" t="inlineStr">
+        <is>
+          <t>0.062</t>
+        </is>
+      </c>
+      <c r="H186" t="inlineStr">
+        <is>
+          <t>-0.081</t>
+        </is>
+      </c>
+      <c r="I186" t="inlineStr">
+        <is>
+          <t>0.049</t>
+        </is>
+      </c>
+      <c r="J186" t="inlineStr">
+        <is>
+          <t>-0.088</t>
+        </is>
+      </c>
+      <c r="K186" t="inlineStr">
+        <is>
+          <t>0.044</t>
+        </is>
+      </c>
+      <c r="L186" t="inlineStr">
+        <is>
+          <t>-0.087</t>
+        </is>
+      </c>
+      <c r="M186" t="inlineStr">
+        <is>
+          <t>0.042</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B187" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C187" t="n">
+        <v>5</v>
+      </c>
+      <c r="D187" t="n">
+        <v>10</v>
+      </c>
+      <c r="E187" t="n">
+        <v>1</v>
+      </c>
+      <c r="F187" t="inlineStr">
+        <is>
+          <t>-0.090</t>
+        </is>
+      </c>
+      <c r="G187" t="inlineStr">
+        <is>
+          <t>0.033</t>
+        </is>
+      </c>
+      <c r="H187" t="inlineStr">
+        <is>
+          <t>-0.087</t>
+        </is>
+      </c>
+      <c r="I187" t="inlineStr">
+        <is>
+          <t>0.051</t>
+        </is>
+      </c>
+      <c r="J187" t="inlineStr">
+        <is>
+          <t>-0.091</t>
+        </is>
+      </c>
+      <c r="K187" t="inlineStr">
+        <is>
+          <t>0.038</t>
+        </is>
+      </c>
+      <c r="L187" t="inlineStr">
+        <is>
+          <t>-0.084</t>
+        </is>
+      </c>
+      <c r="M187" t="inlineStr">
+        <is>
+          <t>0.053</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B188" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C188" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D188" t="n">
+        <v>100</v>
+      </c>
+      <c r="E188" t="n">
+        <v>5</v>
+      </c>
+      <c r="F188" t="inlineStr">
+        <is>
+          <t>-0.076</t>
+        </is>
+      </c>
+      <c r="G188" t="inlineStr">
+        <is>
+          <t>0.062</t>
+        </is>
+      </c>
+      <c r="H188" t="inlineStr">
+        <is>
+          <t>-0.040</t>
+        </is>
+      </c>
+      <c r="I188" t="inlineStr">
+        <is>
+          <t>0.079</t>
+        </is>
+      </c>
+      <c r="J188" t="inlineStr">
+        <is>
+          <t>-0.055</t>
+        </is>
+      </c>
+      <c r="K188" t="inlineStr">
+        <is>
+          <t>0.078</t>
+        </is>
+      </c>
+      <c r="L188" t="inlineStr">
+        <is>
+          <t>-0.051</t>
+        </is>
+      </c>
+      <c r="M188" t="inlineStr">
+        <is>
+          <t>0.079</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B189" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C189" t="n">
+        <v>5</v>
+      </c>
+      <c r="D189" t="n">
+        <v>100</v>
+      </c>
+      <c r="E189" t="n">
+        <v>5</v>
+      </c>
+      <c r="F189" t="inlineStr">
+        <is>
+          <t>-0.086</t>
+        </is>
+      </c>
+      <c r="G189" t="inlineStr">
+        <is>
+          <t>0.035</t>
+        </is>
+      </c>
+      <c r="H189" t="inlineStr">
+        <is>
+          <t>-0.079</t>
+        </is>
+      </c>
+      <c r="I189" t="inlineStr">
+        <is>
+          <t>0.061</t>
+        </is>
+      </c>
+      <c r="J189" t="inlineStr">
+        <is>
+          <t>-0.081</t>
+        </is>
+      </c>
+      <c r="K189" t="inlineStr">
+        <is>
+          <t>0.048</t>
+        </is>
+      </c>
+      <c r="L189" t="inlineStr">
+        <is>
+          <t>-0.060</t>
+        </is>
+      </c>
+      <c r="M189" t="inlineStr">
+        <is>
+          <t>0.076</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B190" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C190" t="n">
+        <v>5</v>
+      </c>
+      <c r="D190" t="n">
+        <v>100</v>
+      </c>
+      <c r="E190" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F190" t="inlineStr">
+        <is>
+          <t>-0.076</t>
+        </is>
+      </c>
+      <c r="G190" t="inlineStr">
+        <is>
+          <t>0.060</t>
+        </is>
+      </c>
+      <c r="H190" t="inlineStr">
+        <is>
+          <t>-0.035</t>
+        </is>
+      </c>
+      <c r="I190" t="inlineStr">
+        <is>
+          <t>0.077</t>
+        </is>
+      </c>
+      <c r="J190" t="inlineStr">
+        <is>
+          <t>-0.042</t>
+        </is>
+      </c>
+      <c r="K190" t="inlineStr">
+        <is>
+          <t>0.073</t>
+        </is>
+      </c>
+      <c r="L190" t="inlineStr">
+        <is>
+          <t>-0.079</t>
+        </is>
+      </c>
+      <c r="M190" t="inlineStr">
+        <is>
+          <t>0.036</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B191" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C191" t="n">
+        <v>5</v>
+      </c>
+      <c r="D191" t="n">
+        <v>100</v>
+      </c>
+      <c r="E191" t="n">
+        <v>1</v>
+      </c>
+      <c r="F191" t="inlineStr">
+        <is>
+          <t>-0.062</t>
+        </is>
+      </c>
+      <c r="G191" t="inlineStr">
+        <is>
+          <t>0.055</t>
+        </is>
+      </c>
+      <c r="H191" t="inlineStr">
+        <is>
+          <t>-0.051</t>
+        </is>
+      </c>
+      <c r="I191" t="inlineStr">
+        <is>
+          <t>0.066</t>
+        </is>
+      </c>
+      <c r="J191" t="inlineStr">
+        <is>
+          <t>-0.066</t>
+        </is>
+      </c>
+      <c r="K191" t="inlineStr">
+        <is>
+          <t>0.058</t>
+        </is>
+      </c>
+      <c r="L191" t="inlineStr">
+        <is>
+          <t>-0.060</t>
+        </is>
+      </c>
+      <c r="M191" t="inlineStr">
+        <is>
+          <t>0.069</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B192" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C192" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D192" t="n">
+        <v>50</v>
+      </c>
+      <c r="E192" t="n">
+        <v>1</v>
+      </c>
+      <c r="F192" t="inlineStr">
+        <is>
+          <t>-0.072</t>
+        </is>
+      </c>
+      <c r="G192" t="inlineStr">
+        <is>
+          <t>0.049</t>
+        </is>
+      </c>
+      <c r="H192" t="inlineStr">
+        <is>
+          <t>-0.064</t>
+        </is>
+      </c>
+      <c r="I192" t="inlineStr">
+        <is>
+          <t>0.056</t>
+        </is>
+      </c>
+      <c r="J192" t="inlineStr">
+        <is>
+          <t>-0.075</t>
+        </is>
+      </c>
+      <c r="K192" t="inlineStr">
+        <is>
+          <t>0.055</t>
+        </is>
+      </c>
+      <c r="L192" t="inlineStr">
+        <is>
+          <t>-0.061</t>
+        </is>
+      </c>
+      <c r="M192" t="inlineStr">
+        <is>
+          <t>0.070</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B193" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C193" t="n">
+        <v>5</v>
+      </c>
+      <c r="D193" t="n">
+        <v>50</v>
+      </c>
+      <c r="E193" t="n">
+        <v>1</v>
+      </c>
+      <c r="F193" t="inlineStr">
+        <is>
+          <t>-0.075</t>
+        </is>
+      </c>
+      <c r="G193" t="inlineStr">
+        <is>
+          <t>0.061</t>
+        </is>
+      </c>
+      <c r="H193" t="inlineStr">
+        <is>
+          <t>-0.070</t>
+        </is>
+      </c>
+      <c r="I193" t="inlineStr">
+        <is>
+          <t>0.054</t>
+        </is>
+      </c>
+      <c r="J193" t="inlineStr">
+        <is>
+          <t>-0.070</t>
+        </is>
+      </c>
+      <c r="K193" t="inlineStr">
+        <is>
+          <t>0.059</t>
+        </is>
+      </c>
+      <c r="L193" t="inlineStr">
+        <is>
+          <t>-0.075</t>
+        </is>
+      </c>
+      <c r="M193" t="inlineStr">
+        <is>
+          <t>0.048</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B194" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C194" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D194" t="n">
+        <v>100</v>
+      </c>
+      <c r="E194" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F194" t="inlineStr">
+        <is>
+          <t>-0.073</t>
+        </is>
+      </c>
+      <c r="G194" t="inlineStr">
+        <is>
+          <t>0.060</t>
+        </is>
+      </c>
+      <c r="H194" t="inlineStr">
+        <is>
+          <t>-0.072</t>
+        </is>
+      </c>
+      <c r="I194" t="inlineStr">
+        <is>
+          <t>0.049</t>
+        </is>
+      </c>
+      <c r="J194" t="inlineStr">
+        <is>
+          <t>-0.071</t>
+        </is>
+      </c>
+      <c r="K194" t="inlineStr">
+        <is>
+          <t>0.055</t>
+        </is>
+      </c>
+      <c r="L194" t="inlineStr">
+        <is>
+          <t>-0.077</t>
+        </is>
+      </c>
+      <c r="M194" t="inlineStr">
+        <is>
+          <t>0.041</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B195" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C195" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D195" t="n">
+        <v>50</v>
+      </c>
+      <c r="E195" t="n">
+        <v>5</v>
+      </c>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>-0.032</t>
+        </is>
+      </c>
+      <c r="G195" t="inlineStr">
+        <is>
+          <t>0.095</t>
+        </is>
+      </c>
+      <c r="H195" t="inlineStr">
+        <is>
+          <t>-0.093</t>
+        </is>
+      </c>
+      <c r="I195" t="inlineStr">
+        <is>
+          <t>0.050</t>
+        </is>
+      </c>
+      <c r="J195" t="inlineStr">
+        <is>
+          <t>-0.089</t>
+        </is>
+      </c>
+      <c r="K195" t="inlineStr">
+        <is>
+          <t>0.041</t>
+        </is>
+      </c>
+      <c r="L195" t="inlineStr">
+        <is>
+          <t>-0.088</t>
+        </is>
+      </c>
+      <c r="M195" t="inlineStr">
+        <is>
+          <t>0.042</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B196" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C196" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D196" t="n">
+        <v>100</v>
+      </c>
+      <c r="E196" t="n">
+        <v>1</v>
+      </c>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>-0.063</t>
+        </is>
+      </c>
+      <c r="G196" t="inlineStr">
+        <is>
+          <t>0.056</t>
+        </is>
+      </c>
+      <c r="H196" t="inlineStr">
+        <is>
+          <t>-0.061</t>
+        </is>
+      </c>
+      <c r="I196" t="inlineStr">
+        <is>
+          <t>0.060</t>
+        </is>
+      </c>
+      <c r="J196" t="inlineStr">
+        <is>
+          <t>-0.057</t>
+        </is>
+      </c>
+      <c r="K196" t="inlineStr">
+        <is>
+          <t>0.062</t>
+        </is>
+      </c>
+      <c r="L196" t="inlineStr">
+        <is>
+          <t>-0.049</t>
+        </is>
+      </c>
+      <c r="M196" t="inlineStr">
+        <is>
+          <t>0.072</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B197" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C197" t="n">
+        <v>5</v>
+      </c>
+      <c r="D197" t="n">
+        <v>50</v>
+      </c>
+      <c r="E197" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>-0.088</t>
+        </is>
+      </c>
+      <c r="G197" t="inlineStr">
+        <is>
+          <t>0.036</t>
+        </is>
+      </c>
+      <c r="H197" t="inlineStr">
+        <is>
+          <t>-0.080</t>
+        </is>
+      </c>
+      <c r="I197" t="inlineStr">
+        <is>
+          <t>0.067</t>
+        </is>
+      </c>
+      <c r="J197" t="inlineStr">
+        <is>
+          <t>-0.058</t>
+        </is>
+      </c>
+      <c r="K197" t="inlineStr">
+        <is>
+          <t>0.072</t>
+        </is>
+      </c>
+      <c r="L197" t="inlineStr">
+        <is>
+          <t>-0.079</t>
+        </is>
+      </c>
+      <c r="M197" t="inlineStr">
+        <is>
+          <t>0.059</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B198" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C198" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D198" t="n">
+        <v>50</v>
+      </c>
+      <c r="E198" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>-0.090</t>
+        </is>
+      </c>
+      <c r="G198" t="inlineStr">
+        <is>
+          <t>0.031</t>
+        </is>
+      </c>
+      <c r="H198" t="inlineStr">
+        <is>
+          <t>-0.072</t>
+        </is>
+      </c>
+      <c r="I198" t="inlineStr">
+        <is>
+          <t>0.060</t>
+        </is>
+      </c>
+      <c r="J198" t="inlineStr">
+        <is>
+          <t>-0.081</t>
+        </is>
+      </c>
+      <c r="K198" t="inlineStr">
+        <is>
+          <t>0.051</t>
+        </is>
+      </c>
+      <c r="L198" t="inlineStr">
+        <is>
+          <t>-0.077</t>
+        </is>
+      </c>
+      <c r="M198" t="inlineStr">
+        <is>
+          <t>0.062</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B199" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C199" t="n">
+        <v>5</v>
+      </c>
+      <c r="D199" t="n">
+        <v>10</v>
+      </c>
+      <c r="E199" t="n">
+        <v>5</v>
+      </c>
+      <c r="F199" t="inlineStr">
+        <is>
+          <t>-0.098</t>
+        </is>
+      </c>
+      <c r="G199" t="inlineStr">
+        <is>
+          <t>0.012</t>
+        </is>
+      </c>
+      <c r="H199" t="inlineStr">
+        <is>
+          <t>-0.099</t>
+        </is>
+      </c>
+      <c r="I199" t="inlineStr">
+        <is>
+          <t>0.007</t>
+        </is>
+      </c>
+      <c r="J199" t="inlineStr">
+        <is>
+          <t>-0.085</t>
+        </is>
+      </c>
+      <c r="K199" t="inlineStr">
+        <is>
+          <t>0.060</t>
+        </is>
+      </c>
+      <c r="L199" t="inlineStr">
+        <is>
+          <t>-0.096</t>
+        </is>
+      </c>
+      <c r="M199" t="inlineStr">
+        <is>
+          <t>0.026</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B200" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C200" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D200" t="n">
+        <v>10</v>
+      </c>
+      <c r="E200" t="n">
+        <v>5</v>
+      </c>
+      <c r="F200" t="inlineStr">
+        <is>
+          <t>-0.094</t>
+        </is>
+      </c>
+      <c r="G200" t="inlineStr">
+        <is>
+          <t>0.038</t>
+        </is>
+      </c>
+      <c r="H200" t="inlineStr">
+        <is>
+          <t>-0.096</t>
+        </is>
+      </c>
+      <c r="I200" t="inlineStr">
+        <is>
+          <t>0.038</t>
+        </is>
+      </c>
+      <c r="J200" t="inlineStr">
+        <is>
+          <t>-0.094</t>
+        </is>
+      </c>
+      <c r="K200" t="inlineStr">
+        <is>
+          <t>0.038</t>
+        </is>
+      </c>
+      <c r="L200" t="inlineStr">
+        <is>
+          <t>-0.089</t>
+        </is>
+      </c>
+      <c r="M200" t="inlineStr">
+        <is>
+          <t>0.044</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B201" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C201" t="n">
+        <v>5</v>
+      </c>
+      <c r="D201" t="n">
+        <v>50</v>
+      </c>
+      <c r="E201" t="n">
+        <v>5</v>
+      </c>
+      <c r="F201" t="inlineStr">
+        <is>
+          <t>-0.095</t>
+        </is>
+      </c>
+      <c r="G201" t="inlineStr">
+        <is>
+          <t>0.029</t>
+        </is>
+      </c>
+      <c r="H201" t="inlineStr">
+        <is>
+          <t>-0.073</t>
+        </is>
+      </c>
+      <c r="I201" t="inlineStr">
+        <is>
+          <t>0.067</t>
+        </is>
+      </c>
+      <c r="J201" t="inlineStr">
+        <is>
+          <t>-0.095</t>
+        </is>
+      </c>
+      <c r="K201" t="inlineStr">
+        <is>
+          <t>0.020</t>
+        </is>
+      </c>
+      <c r="L201" t="inlineStr">
+        <is>
+          <t>-0.085</t>
+        </is>
+      </c>
+      <c r="M201" t="inlineStr">
+        <is>
+          <t>0.054</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B202" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C202" t="n">
+        <v>5</v>
+      </c>
+      <c r="D202" t="n">
+        <v>10</v>
+      </c>
+      <c r="E202" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F202" t="inlineStr">
+        <is>
+          <t>-0.075</t>
+        </is>
+      </c>
+      <c r="G202" t="inlineStr">
+        <is>
+          <t>0.063</t>
+        </is>
+      </c>
+      <c r="H202" t="inlineStr">
+        <is>
+          <t>-0.095</t>
+        </is>
+      </c>
+      <c r="I202" t="inlineStr">
+        <is>
+          <t>0.031</t>
+        </is>
+      </c>
+      <c r="J202" t="inlineStr">
+        <is>
+          <t>-0.099</t>
+        </is>
+      </c>
+      <c r="K202" t="inlineStr">
+        <is>
+          <t>0.005</t>
+        </is>
+      </c>
+      <c r="L202" t="inlineStr">
+        <is>
+          <t>-0.094</t>
+        </is>
+      </c>
+      <c r="M202" t="inlineStr">
+        <is>
+          <t>0.033</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B203" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C203" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D203" t="n">
+        <v>10</v>
+      </c>
+      <c r="E203" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F203" t="inlineStr">
+        <is>
+          <t>-0.095</t>
+        </is>
+      </c>
+      <c r="G203" t="inlineStr">
+        <is>
+          <t>0.021</t>
+        </is>
+      </c>
+      <c r="H203" t="inlineStr">
+        <is>
+          <t>-0.087</t>
+        </is>
+      </c>
+      <c r="I203" t="inlineStr">
+        <is>
+          <t>0.047</t>
+        </is>
+      </c>
+      <c r="J203" t="inlineStr">
+        <is>
+          <t>-0.095</t>
+        </is>
+      </c>
+      <c r="K203" t="inlineStr">
+        <is>
+          <t>0.023</t>
+        </is>
+      </c>
+      <c r="L203" t="inlineStr">
+        <is>
+          <t>-0.095</t>
+        </is>
+      </c>
+      <c r="M203" t="inlineStr">
+        <is>
+          <t>0.028</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B204" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C204" t="n">
+        <v>5</v>
+      </c>
+      <c r="D204" t="n">
+        <v>10</v>
+      </c>
+      <c r="E204" t="n">
+        <v>1</v>
+      </c>
+      <c r="F204" t="inlineStr">
+        <is>
+          <t>-0.084</t>
+        </is>
+      </c>
+      <c r="G204" t="inlineStr">
+        <is>
+          <t>0.044</t>
+        </is>
+      </c>
+      <c r="H204" t="inlineStr">
+        <is>
+          <t>-0.090</t>
+        </is>
+      </c>
+      <c r="I204" t="inlineStr">
+        <is>
+          <t>0.047</t>
+        </is>
+      </c>
+      <c r="J204" t="inlineStr">
+        <is>
+          <t>-0.094</t>
+        </is>
+      </c>
+      <c r="K204" t="inlineStr">
+        <is>
+          <t>0.025</t>
+        </is>
+      </c>
+      <c r="L204" t="inlineStr">
+        <is>
+          <t>-0.092</t>
+        </is>
+      </c>
+      <c r="M204" t="inlineStr">
+        <is>
+          <t>0.027</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B205" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C205" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D205" t="n">
+        <v>10</v>
+      </c>
+      <c r="E205" t="n">
+        <v>1</v>
+      </c>
+      <c r="F205" t="inlineStr">
+        <is>
+          <t>-0.087</t>
+        </is>
+      </c>
+      <c r="G205" t="inlineStr">
+        <is>
+          <t>0.043</t>
+        </is>
+      </c>
+      <c r="H205" t="inlineStr">
+        <is>
+          <t>-0.092</t>
+        </is>
+      </c>
+      <c r="I205" t="inlineStr">
+        <is>
+          <t>0.026</t>
+        </is>
+      </c>
+      <c r="J205" t="inlineStr">
+        <is>
+          <t>-0.091</t>
+        </is>
+      </c>
+      <c r="K205" t="inlineStr">
+        <is>
+          <t>0.028</t>
+        </is>
+      </c>
+      <c r="L205" t="inlineStr">
+        <is>
+          <t>-0.088</t>
+        </is>
+      </c>
+      <c r="M205" t="inlineStr">
+        <is>
+          <t>0.038</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B206" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C206" t="n">
+        <v>1</v>
+      </c>
+      <c r="D206" t="n">
+        <v>100</v>
+      </c>
+      <c r="E206" t="n">
+        <v>5</v>
+      </c>
+      <c r="F206" t="inlineStr">
+        <is>
+          <t>-0.050</t>
+        </is>
+      </c>
+      <c r="G206" t="inlineStr">
+        <is>
+          <t>0.073</t>
+        </is>
+      </c>
+      <c r="H206" t="inlineStr">
+        <is>
+          <t>-0.053</t>
+        </is>
+      </c>
+      <c r="I206" t="inlineStr">
+        <is>
+          <t>0.076</t>
+        </is>
+      </c>
+      <c r="J206" t="inlineStr">
+        <is>
+          <t>-0.083</t>
+        </is>
+      </c>
+      <c r="K206" t="inlineStr">
+        <is>
+          <t>0.044</t>
+        </is>
+      </c>
+      <c r="L206" t="inlineStr">
+        <is>
+          <t>-0.036</t>
+        </is>
+      </c>
+      <c r="M206" t="inlineStr">
+        <is>
+          <t>0.100</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B207" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C207" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D207" t="n">
+        <v>100</v>
+      </c>
+      <c r="E207" t="n">
+        <v>1</v>
+      </c>
+      <c r="F207" t="inlineStr">
+        <is>
+          <t>-0.058</t>
+        </is>
+      </c>
+      <c r="G207" t="inlineStr">
+        <is>
+          <t>0.067</t>
+        </is>
+      </c>
+      <c r="H207" t="inlineStr">
+        <is>
+          <t>-0.060</t>
+        </is>
+      </c>
+      <c r="I207" t="inlineStr">
+        <is>
+          <t>0.059</t>
+        </is>
+      </c>
+      <c r="J207" t="inlineStr">
+        <is>
+          <t>-0.062</t>
+        </is>
+      </c>
+      <c r="K207" t="inlineStr">
+        <is>
+          <t>0.059</t>
+        </is>
+      </c>
+      <c r="L207" t="inlineStr">
+        <is>
+          <t>-0.055</t>
+        </is>
+      </c>
+      <c r="M207" t="inlineStr">
+        <is>
+          <t>0.067</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B208" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C208" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D208" t="n">
+        <v>100</v>
+      </c>
+      <c r="E208" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F208" t="inlineStr">
+        <is>
+          <t>-0.068</t>
+        </is>
+      </c>
+      <c r="G208" t="inlineStr">
+        <is>
+          <t>0.060</t>
+        </is>
+      </c>
+      <c r="H208" t="inlineStr">
+        <is>
+          <t>-0.079</t>
+        </is>
+      </c>
+      <c r="I208" t="inlineStr">
+        <is>
+          <t>0.055</t>
+        </is>
+      </c>
+      <c r="J208" t="inlineStr">
+        <is>
+          <t>-0.079</t>
+        </is>
+      </c>
+      <c r="K208" t="inlineStr">
+        <is>
+          <t>0.042</t>
+        </is>
+      </c>
+      <c r="L208" t="inlineStr">
+        <is>
+          <t>-0.086</t>
+        </is>
+      </c>
+      <c r="M208" t="inlineStr">
+        <is>
+          <t>0.034</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B209" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C209" t="n">
+        <v>1</v>
+      </c>
+      <c r="D209" t="n">
+        <v>50</v>
+      </c>
+      <c r="E209" t="n">
+        <v>5</v>
+      </c>
+      <c r="F209" t="inlineStr">
+        <is>
+          <t>-0.093</t>
+        </is>
+      </c>
+      <c r="G209" t="inlineStr">
+        <is>
+          <t>0.035</t>
+        </is>
+      </c>
+      <c r="H209" t="inlineStr">
+        <is>
+          <t>-0.097</t>
+        </is>
+      </c>
+      <c r="I209" t="inlineStr">
+        <is>
+          <t>0.017</t>
+        </is>
+      </c>
+      <c r="J209" t="inlineStr">
+        <is>
+          <t>-0.091</t>
+        </is>
+      </c>
+      <c r="K209" t="inlineStr">
+        <is>
+          <t>0.038</t>
+        </is>
+      </c>
+      <c r="L209" t="inlineStr">
+        <is>
+          <t>-0.091</t>
+        </is>
+      </c>
+      <c r="M209" t="inlineStr">
+        <is>
+          <t>0.035</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B210" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C210" t="n">
+        <v>1</v>
+      </c>
+      <c r="D210" t="n">
+        <v>100</v>
+      </c>
+      <c r="E210" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F210" t="inlineStr">
+        <is>
+          <t>-0.062</t>
+        </is>
+      </c>
+      <c r="G210" t="inlineStr">
+        <is>
+          <t>0.059</t>
+        </is>
+      </c>
+      <c r="H210" t="inlineStr">
+        <is>
+          <t>-0.082</t>
+        </is>
+      </c>
+      <c r="I210" t="inlineStr">
+        <is>
+          <t>0.038</t>
+        </is>
+      </c>
+      <c r="J210" t="inlineStr">
+        <is>
+          <t>-0.078</t>
+        </is>
+      </c>
+      <c r="K210" t="inlineStr">
+        <is>
+          <t>0.043</t>
+        </is>
+      </c>
+      <c r="L210" t="inlineStr">
+        <is>
+          <t>-0.056</t>
+        </is>
+      </c>
+      <c r="M210" t="inlineStr">
+        <is>
+          <t>0.063</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B211" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C211" t="n">
+        <v>1</v>
+      </c>
+      <c r="D211" t="n">
+        <v>100</v>
+      </c>
+      <c r="E211" t="n">
+        <v>1</v>
+      </c>
+      <c r="F211" t="inlineStr">
+        <is>
+          <t>-0.055</t>
+        </is>
+      </c>
+      <c r="G211" t="inlineStr">
+        <is>
+          <t>0.071</t>
+        </is>
+      </c>
+      <c r="H211" t="inlineStr">
+        <is>
+          <t>-0.058</t>
+        </is>
+      </c>
+      <c r="I211" t="inlineStr">
+        <is>
+          <t>0.067</t>
+        </is>
+      </c>
+      <c r="J211" t="inlineStr">
+        <is>
+          <t>-0.061</t>
+        </is>
+      </c>
+      <c r="K211" t="inlineStr">
+        <is>
+          <t>0.053</t>
+        </is>
+      </c>
+      <c r="L211" t="inlineStr">
+        <is>
+          <t>-0.057</t>
+        </is>
+      </c>
+      <c r="M211" t="inlineStr">
+        <is>
+          <t>0.073</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B212" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C212" t="n">
+        <v>1</v>
+      </c>
+      <c r="D212" t="n">
+        <v>10</v>
+      </c>
+      <c r="E212" t="n">
+        <v>5</v>
+      </c>
+      <c r="F212" t="inlineStr">
+        <is>
+          <t>-0.092</t>
+        </is>
+      </c>
+      <c r="G212" t="inlineStr">
+        <is>
+          <t>0.033</t>
+        </is>
+      </c>
+      <c r="H212" t="inlineStr">
+        <is>
+          <t>-0.098</t>
+        </is>
+      </c>
+      <c r="I212" t="inlineStr">
+        <is>
+          <t>0.015</t>
+        </is>
+      </c>
+      <c r="J212" t="inlineStr">
+        <is>
+          <t>-0.099</t>
+        </is>
+      </c>
+      <c r="K212" t="inlineStr">
+        <is>
+          <t>0.007</t>
+        </is>
+      </c>
+      <c r="L212" t="inlineStr">
+        <is>
+          <t>-0.096</t>
+        </is>
+      </c>
+      <c r="M212" t="inlineStr">
+        <is>
+          <t>0.030</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B213" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C213" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D213" t="n">
+        <v>10</v>
+      </c>
+      <c r="E213" t="n">
+        <v>5</v>
+      </c>
+      <c r="F213" t="inlineStr">
+        <is>
+          <t>-0.096</t>
+        </is>
+      </c>
+      <c r="G213" t="inlineStr">
+        <is>
+          <t>0.023</t>
+        </is>
+      </c>
+      <c r="H213" t="inlineStr">
+        <is>
+          <t>-0.097</t>
+        </is>
+      </c>
+      <c r="I213" t="inlineStr">
+        <is>
+          <t>0.016</t>
+        </is>
+      </c>
+      <c r="J213" t="inlineStr">
+        <is>
+          <t>-0.096</t>
+        </is>
+      </c>
+      <c r="K213" t="inlineStr">
+        <is>
+          <t>0.020</t>
+        </is>
+      </c>
+      <c r="L213" t="inlineStr">
+        <is>
+          <t>-0.098</t>
+        </is>
+      </c>
+      <c r="M213" t="inlineStr">
+        <is>
+          <t>0.024</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B214" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C214" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D214" t="n">
+        <v>50</v>
+      </c>
+      <c r="E214" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F214" t="inlineStr">
+        <is>
+          <t>-0.064</t>
+        </is>
+      </c>
+      <c r="G214" t="inlineStr">
+        <is>
+          <t>0.056</t>
+        </is>
+      </c>
+      <c r="H214" t="inlineStr">
+        <is>
+          <t>-0.093</t>
+        </is>
+      </c>
+      <c r="I214" t="inlineStr">
+        <is>
+          <t>0.024</t>
+        </is>
+      </c>
+      <c r="J214" t="inlineStr">
+        <is>
+          <t>-0.085</t>
+        </is>
+      </c>
+      <c r="K214" t="inlineStr">
+        <is>
+          <t>0.033</t>
+        </is>
+      </c>
+      <c r="L214" t="inlineStr">
+        <is>
+          <t>-0.072</t>
+        </is>
+      </c>
+      <c r="M214" t="inlineStr">
+        <is>
+          <t>0.069</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B215" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C215" t="n">
+        <v>1</v>
+      </c>
+      <c r="D215" t="n">
+        <v>50</v>
+      </c>
+      <c r="E215" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F215" t="inlineStr">
+        <is>
+          <t>-0.070</t>
+        </is>
+      </c>
+      <c r="G215" t="inlineStr">
+        <is>
+          <t>0.050</t>
+        </is>
+      </c>
+      <c r="H215" t="inlineStr">
+        <is>
+          <t>-0.091</t>
+        </is>
+      </c>
+      <c r="I215" t="inlineStr">
+        <is>
+          <t>0.023</t>
+        </is>
+      </c>
+      <c r="J215" t="inlineStr">
+        <is>
+          <t>-0.088</t>
+        </is>
+      </c>
+      <c r="K215" t="inlineStr">
+        <is>
+          <t>0.036</t>
+        </is>
+      </c>
+      <c r="L215" t="inlineStr">
+        <is>
+          <t>-0.090</t>
+        </is>
+      </c>
+      <c r="M215" t="inlineStr">
+        <is>
+          <t>0.025</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B216" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C216" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D216" t="n">
+        <v>100</v>
+      </c>
+      <c r="E216" t="n">
+        <v>5</v>
+      </c>
+      <c r="F216" t="inlineStr">
+        <is>
+          <t>-0.070</t>
+        </is>
+      </c>
+      <c r="G216" t="inlineStr">
+        <is>
+          <t>0.048</t>
+        </is>
+      </c>
+      <c r="H216" t="inlineStr">
+        <is>
+          <t>-0.040</t>
+        </is>
+      </c>
+      <c r="I216" t="inlineStr">
+        <is>
+          <t>0.088</t>
+        </is>
+      </c>
+      <c r="J216" t="inlineStr">
+        <is>
+          <t>-0.085</t>
+        </is>
+      </c>
+      <c r="K216" t="inlineStr">
+        <is>
+          <t>0.044</t>
+        </is>
+      </c>
+      <c r="L216" t="inlineStr">
+        <is>
+          <t>-0.079</t>
+        </is>
+      </c>
+      <c r="M216" t="inlineStr">
+        <is>
+          <t>0.047</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B217" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C217" t="n">
+        <v>1</v>
+      </c>
+      <c r="D217" t="n">
+        <v>50</v>
+      </c>
+      <c r="E217" t="n">
+        <v>1</v>
+      </c>
+      <c r="F217" t="inlineStr">
+        <is>
+          <t>-0.077</t>
+        </is>
+      </c>
+      <c r="G217" t="inlineStr">
+        <is>
+          <t>0.052</t>
+        </is>
+      </c>
+      <c r="H217" t="inlineStr">
+        <is>
+          <t>-0.074</t>
+        </is>
+      </c>
+      <c r="I217" t="inlineStr">
+        <is>
+          <t>0.057</t>
+        </is>
+      </c>
+      <c r="J217" t="inlineStr">
+        <is>
+          <t>-0.073</t>
+        </is>
+      </c>
+      <c r="K217" t="inlineStr">
+        <is>
+          <t>0.054</t>
+        </is>
+      </c>
+      <c r="L217" t="inlineStr">
+        <is>
+          <t>-0.062</t>
+        </is>
+      </c>
+      <c r="M217" t="inlineStr">
+        <is>
+          <t>0.065</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B218" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C218" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D218" t="n">
+        <v>50</v>
+      </c>
+      <c r="E218" t="n">
+        <v>1</v>
+      </c>
+      <c r="F218" t="inlineStr">
+        <is>
+          <t>-0.070</t>
+        </is>
+      </c>
+      <c r="G218" t="inlineStr">
+        <is>
+          <t>0.062</t>
+        </is>
+      </c>
+      <c r="H218" t="inlineStr">
+        <is>
+          <t>-0.074</t>
+        </is>
+      </c>
+      <c r="I218" t="inlineStr">
+        <is>
+          <t>0.056</t>
+        </is>
+      </c>
+      <c r="J218" t="inlineStr">
+        <is>
+          <t>-0.077</t>
+        </is>
+      </c>
+      <c r="K218" t="inlineStr">
+        <is>
+          <t>0.052</t>
+        </is>
+      </c>
+      <c r="L218" t="inlineStr">
+        <is>
+          <t>-0.071</t>
+        </is>
+      </c>
+      <c r="M218" t="inlineStr">
+        <is>
+          <t>0.068</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B219" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C219" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D219" t="n">
+        <v>50</v>
+      </c>
+      <c r="E219" t="n">
+        <v>5</v>
+      </c>
+      <c r="F219" t="inlineStr">
+        <is>
+          <t>-0.093</t>
+        </is>
+      </c>
+      <c r="G219" t="inlineStr">
+        <is>
+          <t>0.030</t>
+        </is>
+      </c>
+      <c r="H219" t="inlineStr">
+        <is>
+          <t>-0.075</t>
+        </is>
+      </c>
+      <c r="I219" t="inlineStr">
+        <is>
+          <t>0.070</t>
+        </is>
+      </c>
+      <c r="J219" t="inlineStr">
+        <is>
+          <t>-0.092</t>
+        </is>
+      </c>
+      <c r="K219" t="inlineStr">
+        <is>
+          <t>0.042</t>
+        </is>
+      </c>
+      <c r="L219" t="inlineStr">
+        <is>
+          <t>-0.092</t>
+        </is>
+      </c>
+      <c r="M219" t="inlineStr">
+        <is>
+          <t>0.041</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B220" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C220" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D220" t="n">
+        <v>10</v>
+      </c>
+      <c r="E220" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F220" t="inlineStr">
+        <is>
+          <t>-0.084</t>
+        </is>
+      </c>
+      <c r="G220" t="inlineStr">
+        <is>
+          <t>0.045</t>
+        </is>
+      </c>
+      <c r="H220" t="inlineStr">
+        <is>
+          <t>-0.095</t>
+        </is>
+      </c>
+      <c r="I220" t="inlineStr">
+        <is>
+          <t>0.020</t>
+        </is>
+      </c>
+      <c r="J220" t="inlineStr">
+        <is>
+          <t>-0.096</t>
+        </is>
+      </c>
+      <c r="K220" t="inlineStr">
+        <is>
+          <t>0.022</t>
+        </is>
+      </c>
+      <c r="L220" t="inlineStr">
+        <is>
+          <t>-0.095</t>
+        </is>
+      </c>
+      <c r="M220" t="inlineStr">
+        <is>
+          <t>0.026</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B221" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C221" t="n">
+        <v>1</v>
+      </c>
+      <c r="D221" t="n">
+        <v>10</v>
+      </c>
+      <c r="E221" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F221" t="inlineStr">
+        <is>
+          <t>-0.081</t>
+        </is>
+      </c>
+      <c r="G221" t="inlineStr">
+        <is>
+          <t>0.041</t>
+        </is>
+      </c>
+      <c r="H221" t="inlineStr">
+        <is>
+          <t>-0.096</t>
+        </is>
+      </c>
+      <c r="I221" t="inlineStr">
+        <is>
+          <t>0.024</t>
+        </is>
+      </c>
+      <c r="J221" t="inlineStr">
+        <is>
+          <t>-0.097</t>
+        </is>
+      </c>
+      <c r="K221" t="inlineStr">
+        <is>
+          <t>0.014</t>
+        </is>
+      </c>
+      <c r="L221" t="inlineStr">
+        <is>
+          <t>-0.095</t>
+        </is>
+      </c>
+      <c r="M221" t="inlineStr">
+        <is>
+          <t>0.021</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B222" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C222" t="n">
+        <v>1</v>
+      </c>
+      <c r="D222" t="n">
+        <v>10</v>
+      </c>
+      <c r="E222" t="n">
+        <v>1</v>
+      </c>
+      <c r="F222" t="inlineStr">
+        <is>
+          <t>-0.083</t>
+        </is>
+      </c>
+      <c r="G222" t="inlineStr">
+        <is>
+          <t>0.042</t>
+        </is>
+      </c>
+      <c r="H222" t="inlineStr">
+        <is>
+          <t>-0.094</t>
+        </is>
+      </c>
+      <c r="I222" t="inlineStr">
+        <is>
+          <t>0.019</t>
+        </is>
+      </c>
+      <c r="J222" t="inlineStr">
+        <is>
+          <t>-0.091</t>
+        </is>
+      </c>
+      <c r="K222" t="inlineStr">
+        <is>
+          <t>0.032</t>
+        </is>
+      </c>
+      <c r="L222" t="inlineStr">
+        <is>
+          <t>-0.088</t>
+        </is>
+      </c>
+      <c r="M222" t="inlineStr">
+        <is>
+          <t>0.038</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B223" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C223" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D223" t="n">
+        <v>10</v>
+      </c>
+      <c r="E223" t="n">
+        <v>1</v>
+      </c>
+      <c r="F223" t="inlineStr">
+        <is>
+          <t>-0.091</t>
+        </is>
+      </c>
+      <c r="G223" t="inlineStr">
+        <is>
+          <t>0.036</t>
+        </is>
+      </c>
+      <c r="H223" t="inlineStr">
+        <is>
+          <t>-0.087</t>
+        </is>
+      </c>
+      <c r="I223" t="inlineStr">
+        <is>
+          <t>0.045</t>
+        </is>
+      </c>
+      <c r="J223" t="inlineStr">
+        <is>
+          <t>-0.091</t>
+        </is>
+      </c>
+      <c r="K223" t="inlineStr">
+        <is>
+          <t>0.038</t>
+        </is>
+      </c>
+      <c r="L223" t="inlineStr">
+        <is>
+          <t>-0.084</t>
+        </is>
+      </c>
+      <c r="M223" t="inlineStr">
+        <is>
+          <t>0.054</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B224" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C224" t="n">
+        <v>5</v>
+      </c>
+      <c r="D224" t="n">
+        <v>100</v>
+      </c>
+      <c r="E224" t="n">
+        <v>1</v>
+      </c>
+      <c r="F224" t="inlineStr">
+        <is>
+          <t>-0.065</t>
+        </is>
+      </c>
+      <c r="G224" t="inlineStr">
+        <is>
+          <t>0.046</t>
+        </is>
+      </c>
+      <c r="H224" t="inlineStr">
+        <is>
+          <t>-0.063</t>
+        </is>
+      </c>
+      <c r="I224" t="inlineStr">
+        <is>
+          <t>0.062</t>
+        </is>
+      </c>
+      <c r="J224" t="inlineStr">
+        <is>
+          <t>-0.057</t>
+        </is>
+      </c>
+      <c r="K224" t="inlineStr">
+        <is>
+          <t>0.063</t>
+        </is>
+      </c>
+      <c r="L224" t="inlineStr">
+        <is>
+          <t>-0.063</t>
+        </is>
+      </c>
+      <c r="M224" t="inlineStr">
+        <is>
+          <t>0.059</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B225" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C225" t="n">
+        <v>5</v>
+      </c>
+      <c r="D225" t="n">
+        <v>100</v>
+      </c>
+      <c r="E225" t="n">
+        <v>5</v>
+      </c>
+      <c r="F225" t="inlineStr">
+        <is>
+          <t>-0.088</t>
+        </is>
+      </c>
+      <c r="G225" t="inlineStr">
+        <is>
+          <t>0.035</t>
+        </is>
+      </c>
+      <c r="H225" t="inlineStr">
+        <is>
+          <t>-0.085</t>
+        </is>
+      </c>
+      <c r="I225" t="inlineStr">
+        <is>
+          <t>0.040</t>
+        </is>
+      </c>
+      <c r="J225" t="inlineStr">
+        <is>
+          <t>-0.085</t>
+        </is>
+      </c>
+      <c r="K225" t="inlineStr">
+        <is>
+          <t>0.052</t>
+        </is>
+      </c>
+      <c r="L225" t="inlineStr">
+        <is>
+          <t>-0.084</t>
+        </is>
+      </c>
+      <c r="M225" t="inlineStr">
+        <is>
+          <t>0.044</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B226" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C226" t="n">
+        <v>5</v>
+      </c>
+      <c r="D226" t="n">
+        <v>50</v>
+      </c>
+      <c r="E226" t="n">
+        <v>5</v>
+      </c>
+      <c r="F226" t="inlineStr">
+        <is>
+          <t>-0.094</t>
+        </is>
+      </c>
+      <c r="G226" t="inlineStr">
+        <is>
+          <t>0.037</t>
+        </is>
+      </c>
+      <c r="H226" t="inlineStr">
+        <is>
+          <t>-0.059</t>
+        </is>
+      </c>
+      <c r="I226" t="inlineStr">
+        <is>
+          <t>0.074</t>
+        </is>
+      </c>
+      <c r="J226" t="inlineStr">
+        <is>
+          <t>-0.060</t>
+        </is>
+      </c>
+      <c r="K226" t="inlineStr">
+        <is>
+          <t>0.092</t>
+        </is>
+      </c>
+      <c r="L226" t="inlineStr">
+        <is>
+          <t>-0.092</t>
+        </is>
+      </c>
+      <c r="M226" t="inlineStr">
+        <is>
+          <t>0.037</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B227" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C227" t="n">
+        <v>5</v>
+      </c>
+      <c r="D227" t="n">
+        <v>100</v>
+      </c>
+      <c r="E227" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F227" t="inlineStr">
+        <is>
+          <t>-0.072</t>
+        </is>
+      </c>
+      <c r="G227" t="inlineStr">
+        <is>
+          <t>0.052</t>
+        </is>
+      </c>
+      <c r="H227" t="inlineStr">
+        <is>
+          <t>-0.069</t>
+        </is>
+      </c>
+      <c r="I227" t="inlineStr">
+        <is>
+          <t>0.060</t>
+        </is>
+      </c>
+      <c r="J227" t="inlineStr">
+        <is>
+          <t>-0.083</t>
+        </is>
+      </c>
+      <c r="K227" t="inlineStr">
+        <is>
+          <t>0.038</t>
+        </is>
+      </c>
+      <c r="L227" t="inlineStr">
+        <is>
+          <t>-0.076</t>
+        </is>
+      </c>
+      <c r="M227" t="inlineStr">
+        <is>
+          <t>0.055</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B228" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C228" t="n">
+        <v>5</v>
+      </c>
+      <c r="D228" t="n">
+        <v>10</v>
+      </c>
+      <c r="E228" t="n">
+        <v>5</v>
+      </c>
+      <c r="F228" t="inlineStr">
+        <is>
+          <t>0.024</t>
+        </is>
+      </c>
+      <c r="G228" t="inlineStr">
+        <is>
+          <t>0.103</t>
+        </is>
+      </c>
+      <c r="H228" t="inlineStr">
+        <is>
+          <t>-0.098</t>
+        </is>
+      </c>
+      <c r="I228" t="inlineStr">
+        <is>
+          <t>0.013</t>
+        </is>
+      </c>
+      <c r="J228" t="inlineStr">
+        <is>
+          <t>-0.098</t>
+        </is>
+      </c>
+      <c r="K228" t="inlineStr">
+        <is>
+          <t>0.018</t>
+        </is>
+      </c>
+      <c r="L228" t="inlineStr">
+        <is>
+          <t>-0.098</t>
+        </is>
+      </c>
+      <c r="M228" t="inlineStr">
+        <is>
+          <t>0.009</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B229" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C229" t="n">
+        <v>5</v>
+      </c>
+      <c r="D229" t="n">
+        <v>10</v>
+      </c>
+      <c r="E229" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F229" t="inlineStr">
+        <is>
+          <t>-0.078</t>
+        </is>
+      </c>
+      <c r="G229" t="inlineStr">
+        <is>
+          <t>0.060</t>
+        </is>
+      </c>
+      <c r="H229" t="inlineStr">
+        <is>
+          <t>-0.095</t>
+        </is>
+      </c>
+      <c r="I229" t="inlineStr">
+        <is>
+          <t>0.025</t>
+        </is>
+      </c>
+      <c r="J229" t="inlineStr">
+        <is>
+          <t>-0.095</t>
+        </is>
+      </c>
+      <c r="K229" t="inlineStr">
+        <is>
+          <t>0.022</t>
+        </is>
+      </c>
+      <c r="L229" t="inlineStr">
+        <is>
+          <t>-0.096</t>
+        </is>
+      </c>
+      <c r="M229" t="inlineStr">
+        <is>
+          <t>0.017</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B230" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C230" t="n">
+        <v>5</v>
+      </c>
+      <c r="D230" t="n">
+        <v>50</v>
+      </c>
+      <c r="E230" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F230" t="inlineStr">
+        <is>
+          <t>-0.091</t>
+        </is>
+      </c>
+      <c r="G230" t="inlineStr">
+        <is>
+          <t>0.029</t>
+        </is>
+      </c>
+      <c r="H230" t="inlineStr">
+        <is>
+          <t>-0.085</t>
+        </is>
+      </c>
+      <c r="I230" t="inlineStr">
+        <is>
+          <t>0.045</t>
+        </is>
+      </c>
+      <c r="J230" t="inlineStr">
+        <is>
+          <t>-0.090</t>
+        </is>
+      </c>
+      <c r="K230" t="inlineStr">
+        <is>
+          <t>0.033</t>
+        </is>
+      </c>
+      <c r="L230" t="inlineStr">
+        <is>
+          <t>-0.087</t>
+        </is>
+      </c>
+      <c r="M230" t="inlineStr">
+        <is>
+          <t>0.044</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B231" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C231" t="n">
+        <v>5</v>
+      </c>
+      <c r="D231" t="n">
+        <v>50</v>
+      </c>
+      <c r="E231" t="n">
+        <v>1</v>
+      </c>
+      <c r="F231" t="inlineStr">
+        <is>
+          <t>-0.069</t>
+        </is>
+      </c>
+      <c r="G231" t="inlineStr">
+        <is>
+          <t>0.056</t>
+        </is>
+      </c>
+      <c r="H231" t="inlineStr">
+        <is>
+          <t>-0.081</t>
+        </is>
+      </c>
+      <c r="I231" t="inlineStr">
+        <is>
+          <t>0.040</t>
+        </is>
+      </c>
+      <c r="J231" t="inlineStr">
+        <is>
+          <t>-0.077</t>
+        </is>
+      </c>
+      <c r="K231" t="inlineStr">
+        <is>
+          <t>0.049</t>
+        </is>
+      </c>
+      <c r="L231" t="inlineStr">
+        <is>
+          <t>-0.079</t>
+        </is>
+      </c>
+      <c r="M231" t="inlineStr">
+        <is>
+          <t>0.047</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>world3Cont</t>
+        </is>
+      </c>
+      <c r="B232" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C232" t="n">
+        <v>5</v>
+      </c>
+      <c r="D232" t="n">
+        <v>10</v>
+      </c>
+      <c r="E232" t="n">
+        <v>1</v>
+      </c>
+      <c r="F232" t="inlineStr">
+        <is>
+          <t>-0.093</t>
+        </is>
+      </c>
+      <c r="G232" t="inlineStr">
+        <is>
+          <t>0.024</t>
+        </is>
+      </c>
+      <c r="H232" t="inlineStr">
+        <is>
+          <t>-0.089</t>
+        </is>
+      </c>
+      <c r="I232" t="inlineStr">
+        <is>
+          <t>0.047</t>
+        </is>
+      </c>
+      <c r="J232" t="inlineStr">
+        <is>
+          <t>-0.089</t>
+        </is>
+      </c>
+      <c r="K232" t="inlineStr">
+        <is>
+          <t>0.037</t>
+        </is>
+      </c>
+      <c r="L232" t="inlineStr">
+        <is>
+          <t>-0.091</t>
+        </is>
+      </c>
+      <c r="M232" t="inlineStr">
+        <is>
+          <t>0.029</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>

</xml_diff>